<commit_message>
FIND LARGE AND FIND SMALL
</commit_message>
<xml_diff>
--- a/INSTRUCTIONS/Binary Instructions.xlsx
+++ b/INSTRUCTIONS/Binary Instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="188">
   <si>
     <t>0001</t>
   </si>
@@ -582,7 +582,13 @@
     <t>STRIG</t>
   </si>
   <si>
-    <t>0010110</t>
+    <t>1000000</t>
+  </si>
+  <si>
+    <t>0010000</t>
+  </si>
+  <si>
+    <t>0010001</t>
   </si>
 </sst>
 </file>
@@ -701,17 +707,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1011,7 +1007,7 @@
   <dimension ref="A1:AO101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,13 +1336,13 @@
         <v>16</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>180</v>
+        <v>3</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4" s="16" t="s">
         <v>83</v>
@@ -1355,26 +1351,26 @@
         <v>68</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="J4" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>26010301</v>
+        <v>4C090200</v>
       </c>
       <c r="M4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C4,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0100</v>
+        <v>1001</v>
       </c>
       <c r="N4" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D4,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D4,'HEX GEN BACKEND'!G:G,0)),D4)</f>
-        <v>0000000</v>
+        <v>0000010</v>
       </c>
       <c r="O4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E4,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P4" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F4,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F4,'HEX GEN BACKEND'!H:H,0)),F4)</f>
@@ -1386,23 +1382,23 @@
       </c>
       <c r="R4" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H4,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H4,'HEX GEN BACKEND'!I:I,0)),H4)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="S4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I4,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>00</v>
       </c>
       <c r="U4" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00100110000000010000001100000001</v>
+        <v>01001100000010010000001000000000</v>
       </c>
       <c r="W4" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="X4" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>0110</v>
+        <v>1100</v>
       </c>
       <c r="Y4" s="21" t="str">
         <f t="shared" si="4"/>
@@ -1410,7 +1406,7 @@
       </c>
       <c r="Z4" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>1001</v>
       </c>
       <c r="AA4" s="21" t="str">
         <f t="shared" si="6"/>
@@ -1418,7 +1414,7 @@
       </c>
       <c r="AB4" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0010</v>
       </c>
       <c r="AC4" s="21" t="str">
         <f t="shared" si="8"/>
@@ -1426,15 +1422,15 @@
       </c>
       <c r="AD4" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AF4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>C</v>
       </c>
       <c r="AH4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y4,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1442,7 +1438,7 @@
       </c>
       <c r="AI4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="AJ4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA4,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1450,7 +1446,7 @@
       </c>
       <c r="AK4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC4,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1458,11 +1454,11 @@
       </c>
       <c r="AM4" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO4" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>26010301</v>
+        <v>4C090200</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -1476,26 +1472,26 @@
         <v>3</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>98</v>
+        <v>185</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>67</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="J5" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>48020281</v>
+        <v>4F020400</v>
       </c>
       <c r="M5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C5,'HEX GEN BACKEND'!A:A,0))</f>
@@ -1503,15 +1499,15 @@
       </c>
       <c r="N5" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D5,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D5,'HEX GEN BACKEND'!G:G,0)),D5)</f>
-        <v>0000000</v>
+        <v>1000000</v>
       </c>
       <c r="O5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="P5" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F5,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F5,'HEX GEN BACKEND'!H:H,0)),F5)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G5,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1519,15 +1515,15 @@
       </c>
       <c r="R5" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H5,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H5,'HEX GEN BACKEND'!I:I,0)),H5)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="S5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="U5" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000100000001010000001</v>
+        <v>01001111000000100000010000000000</v>
       </c>
       <c r="W5" s="21" t="str">
         <f t="shared" si="2"/>
@@ -1535,7 +1531,7 @@
       </c>
       <c r="X5" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>1111</v>
       </c>
       <c r="Y5" s="21" t="str">
         <f t="shared" si="4"/>
@@ -1551,15 +1547,15 @@
       </c>
       <c r="AB5" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="AC5" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD5" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AF5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W5,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1567,7 +1563,7 @@
       </c>
       <c r="AG5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>F</v>
       </c>
       <c r="AH5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y5,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1583,19 +1579,19 @@
       </c>
       <c r="AK5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AL5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM5" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO5" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>48020281</v>
+        <v>4F020400</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
@@ -1606,49 +1602,49 @@
         <v>16</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>3</v>
+        <v>177</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>69</v>
       </c>
       <c r="J6" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>4C080181</v>
+        <v>0A050501</v>
       </c>
       <c r="M6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C6,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>0001</v>
       </c>
       <c r="N6" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D6,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D6,'HEX GEN BACKEND'!G:G,0)),D6)</f>
-        <v>0000010</v>
+        <v>0000001</v>
       </c>
       <c r="O6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E6,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="P6" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F6,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F6,'HEX GEN BACKEND'!H:H,0)),F6)</f>
-        <v>0000000</v>
+        <v>0000010</v>
       </c>
       <c r="Q6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G6,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="R6" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H6,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H6,'HEX GEN BACKEND'!I:I,0)),H6)</f>
@@ -1656,19 +1652,19 @@
       </c>
       <c r="S6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I6,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U6" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001100000010000000000110000001</v>
+        <v>00001010000001010000010100000001</v>
       </c>
       <c r="W6" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="X6" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>1010</v>
       </c>
       <c r="Y6" s="21" t="str">
         <f t="shared" si="4"/>
@@ -1676,7 +1672,7 @@
       </c>
       <c r="Z6" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0101</v>
       </c>
       <c r="AA6" s="21" t="str">
         <f t="shared" si="6"/>
@@ -1684,11 +1680,11 @@
       </c>
       <c r="AB6" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0001</v>
+        <v>0101</v>
       </c>
       <c r="AC6" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD6" s="21" t="str">
         <f t="shared" si="9"/>
@@ -1696,11 +1692,11 @@
       </c>
       <c r="AF6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="AH6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1708,7 +1704,7 @@
       </c>
       <c r="AI6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AJ6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1716,11 +1712,11 @@
       </c>
       <c r="AK6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AL6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1728,7 +1724,7 @@
       </c>
       <c r="AO6" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>4C080181</v>
+        <v>0A050501</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
@@ -1739,7 +1735,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>77</v>
@@ -1748,24 +1744,24 @@
         <v>68</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>68</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>67</v>
       </c>
       <c r="J7" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>2A090301</v>
+        <v>0A090502</v>
       </c>
       <c r="M7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C7,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0101</v>
+        <v>0001</v>
       </c>
       <c r="N7" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D7,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D7,'HEX GEN BACKEND'!G:G,0)),D7)</f>
@@ -1777,7 +1773,7 @@
       </c>
       <c r="P7" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F7,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F7,'HEX GEN BACKEND'!H:H,0)),F7)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G7,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1785,7 +1781,7 @@
       </c>
       <c r="R7" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H7,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H7,'HEX GEN BACKEND'!I:I,0)),H7)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="S7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I7,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1793,11 +1789,11 @@
       </c>
       <c r="U7" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00101010000010010000001100000001</v>
+        <v>00001010000010010000010100000010</v>
       </c>
       <c r="W7" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="X7" s="21" t="str">
         <f t="shared" si="3"/>
@@ -1817,7 +1813,7 @@
       </c>
       <c r="AB7" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0101</v>
       </c>
       <c r="AC7" s="21" t="str">
         <f t="shared" si="8"/>
@@ -1825,11 +1821,11 @@
       </c>
       <c r="AD7" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0010</v>
       </c>
       <c r="AF7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X7,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1849,7 +1845,7 @@
       </c>
       <c r="AK7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AL7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC7,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1857,11 +1853,11 @@
       </c>
       <c r="AM7" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO7" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>2A090301</v>
+        <v>0A090502</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
@@ -1872,69 +1868,69 @@
         <v>16</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>177</v>
+        <v>3</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="J8" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>0A090302</v>
+        <v>4C0C0081</v>
       </c>
       <c r="M8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C8,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0001</v>
+        <v>1001</v>
       </c>
       <c r="N8" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D8,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D8,'HEX GEN BACKEND'!G:G,0)),D8)</f>
-        <v>0000010</v>
+        <v>0000011</v>
       </c>
       <c r="O8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>10</v>
       </c>
       <c r="P8" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F8,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F8,'HEX GEN BACKEND'!H:H,0)),F8)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="Q8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="R8" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H8,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H8,'HEX GEN BACKEND'!I:I,0)),H8)</f>
-        <v>0000010</v>
+        <v>0000001</v>
       </c>
       <c r="S8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="U8" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00001010000010010000001100000010</v>
+        <v>01001100000011000000000010000001</v>
       </c>
       <c r="W8" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="X8" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="Y8" s="21" t="str">
         <f t="shared" si="4"/>
@@ -1942,7 +1938,7 @@
       </c>
       <c r="Z8" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>1001</v>
+        <v>1100</v>
       </c>
       <c r="AA8" s="21" t="str">
         <f t="shared" si="6"/>
@@ -1950,23 +1946,23 @@
       </c>
       <c r="AB8" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AC8" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD8" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AF8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AG8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="AH8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y8,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1974,7 +1970,7 @@
       </c>
       <c r="AI8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>9</v>
+        <v>C</v>
       </c>
       <c r="AJ8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA8,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1982,19 +1978,19 @@
       </c>
       <c r="AK8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM8" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO8" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>0A090302</v>
+        <v>4C0C0081</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
@@ -2008,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>67</v>
@@ -2020,14 +2016,14 @@
         <v>98</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>68</v>
       </c>
       <c r="J9" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>4C080081</v>
+        <v>4C100082</v>
       </c>
       <c r="M9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C9,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2035,7 +2031,7 @@
       </c>
       <c r="N9" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D9,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D9,'HEX GEN BACKEND'!G:G,0)),D9)</f>
-        <v>0000010</v>
+        <v>0000100</v>
       </c>
       <c r="O9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E9,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2051,7 +2047,7 @@
       </c>
       <c r="R9" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H9,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H9,'HEX GEN BACKEND'!I:I,0)),H9)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="S9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I9,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2059,7 +2055,7 @@
       </c>
       <c r="U9" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001100000010000000000010000001</v>
+        <v>01001100000100000000000010000010</v>
       </c>
       <c r="W9" s="21" t="str">
         <f t="shared" si="2"/>
@@ -2071,11 +2067,11 @@
       </c>
       <c r="Y9" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="Z9" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AA9" s="21" t="str">
         <f t="shared" si="6"/>
@@ -2091,7 +2087,7 @@
       </c>
       <c r="AD9" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0010</v>
       </c>
       <c r="AF9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W9,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2103,11 +2099,11 @@
       </c>
       <c r="AH9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AJ9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA9,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2123,11 +2119,11 @@
       </c>
       <c r="AM9" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO9" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>4C080081</v>
+        <v>4C100082</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
@@ -2138,69 +2134,69 @@
         <v>16</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>3</v>
+        <v>182</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G10" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="J10" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>48020282</v>
+        <v>320D0501</v>
       </c>
       <c r="M10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C10,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>0110</v>
       </c>
       <c r="N10" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D10,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D10,'HEX GEN BACKEND'!G:G,0)),D10)</f>
-        <v>0000000</v>
+        <v>0000011</v>
       </c>
       <c r="O10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="P10" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F10,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F10,'HEX GEN BACKEND'!H:H,0)),F10)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="R10" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H10,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H10,'HEX GEN BACKEND'!I:I,0)),H10)</f>
-        <v>0000010</v>
+        <v>0000001</v>
       </c>
       <c r="S10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>10</v>
       </c>
       <c r="U10" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000100000001010000010</v>
+        <v>00110010000011010000010100000001</v>
       </c>
       <c r="W10" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0011</v>
       </c>
       <c r="X10" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="Y10" s="21" t="str">
         <f t="shared" si="4"/>
@@ -2208,7 +2204,7 @@
       </c>
       <c r="Z10" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0010</v>
+        <v>1101</v>
       </c>
       <c r="AA10" s="21" t="str">
         <f t="shared" si="6"/>
@@ -2216,23 +2212,23 @@
       </c>
       <c r="AB10" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0101</v>
       </c>
       <c r="AC10" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD10" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AF10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y10,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2240,7 +2236,7 @@
       </c>
       <c r="AI10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>D</v>
       </c>
       <c r="AJ10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA10,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2248,19 +2244,19 @@
       </c>
       <c r="AK10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AL10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM10" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO10" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>48020282</v>
+        <v>320D0501</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
@@ -2271,16 +2267,16 @@
         <v>16</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>68</v>
@@ -2293,23 +2289,23 @@
       </c>
       <c r="J11" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>38010302</v>
+        <v>32110502</v>
       </c>
       <c r="M11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C11,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0111</v>
+        <v>0110</v>
       </c>
       <c r="N11" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D11,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D11,'HEX GEN BACKEND'!G:G,0)),D11)</f>
-        <v>0000000</v>
+        <v>0000100</v>
       </c>
       <c r="O11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E11,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="P11" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F11,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F11,'HEX GEN BACKEND'!H:H,0)),F11)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G11,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2325,7 +2321,7 @@
       </c>
       <c r="U11" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00111000000000010000001100000010</v>
+        <v>00110010000100010000010100000010</v>
       </c>
       <c r="W11" s="21" t="str">
         <f t="shared" si="2"/>
@@ -2333,11 +2329,11 @@
       </c>
       <c r="X11" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="Y11" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="Z11" s="21" t="str">
         <f t="shared" si="5"/>
@@ -2349,7 +2345,7 @@
       </c>
       <c r="AB11" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0101</v>
       </c>
       <c r="AC11" s="21" t="str">
         <f t="shared" si="8"/>
@@ -2365,11 +2361,11 @@
       </c>
       <c r="AG11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2381,7 +2377,7 @@
       </c>
       <c r="AK11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AL11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2393,7 +2389,7 @@
       </c>
       <c r="AO11" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>38010302</v>
+        <v>32110502</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -2404,53 +2400,53 @@
         <v>16</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>98</v>
+        <v>172</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>68</v>
       </c>
       <c r="J12" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>48020282</v>
+        <v>562F1881</v>
       </c>
       <c r="M12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C12,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="N12" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D12,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D12,'HEX GEN BACKEND'!G:G,0)),D12)</f>
-        <v>0000000</v>
+        <v>0001011</v>
       </c>
       <c r="O12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E12,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="P12" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F12,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F12,'HEX GEN BACKEND'!H:H,0)),F12)</f>
-        <v>0000001</v>
+        <v>0001100</v>
       </c>
       <c r="Q12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G12,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="R12" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H12,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H12,'HEX GEN BACKEND'!I:I,0)),H12)</f>
-        <v>0000010</v>
+        <v>0000001</v>
       </c>
       <c r="S12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I12,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2458,31 +2454,31 @@
       </c>
       <c r="U12" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000100000001010000010</v>
+        <v>01010110001011110001100010000001</v>
       </c>
       <c r="W12" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0101</v>
       </c>
       <c r="X12" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0110</v>
       </c>
       <c r="Y12" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="Z12" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0010</v>
+        <v>1111</v>
       </c>
       <c r="AA12" s="21" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AB12" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>1000</v>
       </c>
       <c r="AC12" s="21" t="str">
         <f t="shared" si="8"/>
@@ -2490,31 +2486,31 @@
       </c>
       <c r="AD12" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AF12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AG12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AH12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>F</v>
       </c>
       <c r="AJ12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AL12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC12,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2522,11 +2518,11 @@
       </c>
       <c r="AM12" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO12" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>48020282</v>
+        <v>562F1881</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
@@ -2537,37 +2533,37 @@
         <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>182</v>
+        <v>1</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>98</v>
+        <v>174</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>69</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="G13" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="J13" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>36010301</v>
+        <v>56372282</v>
       </c>
       <c r="M13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C13,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0110</v>
+        <v>1010</v>
       </c>
       <c r="N13" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D13,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D13,'HEX GEN BACKEND'!G:G,0)),D13)</f>
-        <v>0000000</v>
+        <v>0001101</v>
       </c>
       <c r="O13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E13,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2575,27 +2571,27 @@
       </c>
       <c r="P13" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F13,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F13,'HEX GEN BACKEND'!H:H,0)),F13)</f>
-        <v>0000001</v>
+        <v>0010001</v>
       </c>
       <c r="Q13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>11</v>
       </c>
       <c r="R13" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H13,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H13,'HEX GEN BACKEND'!I:I,0)),H13)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="S13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="U13" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00110110000000010000001100000001</v>
+        <v>01010110001101110010001010000010</v>
       </c>
       <c r="W13" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0011</v>
+        <v>0101</v>
       </c>
       <c r="X13" s="21" t="str">
         <f t="shared" si="3"/>
@@ -2603,31 +2599,31 @@
       </c>
       <c r="Y13" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="Z13" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0111</v>
       </c>
       <c r="AA13" s="21" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AB13" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0010</v>
       </c>
       <c r="AC13" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD13" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0010</v>
       </c>
       <c r="AF13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X13,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2635,31 +2631,31 @@
       </c>
       <c r="AH13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AJ13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM13" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO13" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>36010301</v>
+        <v>56372282</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
@@ -2673,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>69</v>
@@ -2685,14 +2681,14 @@
         <v>69</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>68</v>
       </c>
       <c r="J14" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>56171A81</v>
+        <v>56431A82</v>
       </c>
       <c r="M14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C14,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2700,7 +2696,7 @@
       </c>
       <c r="N14" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D14,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D14,'HEX GEN BACKEND'!G:G,0)),D14)</f>
-        <v>0000101</v>
+        <v>0010000</v>
       </c>
       <c r="O14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E14,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2716,7 +2712,7 @@
       </c>
       <c r="R14" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H14,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H14,'HEX GEN BACKEND'!I:I,0)),H14)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="S14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I14,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2724,7 +2720,7 @@
       </c>
       <c r="U14" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01010110000101110001101010000001</v>
+        <v>01010110010000110001101010000010</v>
       </c>
       <c r="W14" s="21" t="str">
         <f t="shared" si="2"/>
@@ -2736,11 +2732,11 @@
       </c>
       <c r="Y14" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0001</v>
+        <v>0100</v>
       </c>
       <c r="Z14" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0111</v>
+        <v>0011</v>
       </c>
       <c r="AA14" s="21" t="str">
         <f t="shared" si="6"/>
@@ -2756,7 +2752,7 @@
       </c>
       <c r="AD14" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0010</v>
       </c>
       <c r="AF14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W14,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2768,11 +2764,11 @@
       </c>
       <c r="AH14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AI14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AJ14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA14,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2788,11 +2784,11 @@
       </c>
       <c r="AM14" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO14" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>56171A81</v>
+        <v>56431A82</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -2803,61 +2799,61 @@
         <v>16</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>3</v>
+        <v>184</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="17" t="s">
+      <c r="H15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>98</v>
       </c>
       <c r="J15" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>4A0A0200</v>
+        <v>40010503</v>
       </c>
       <c r="M15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C15,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="N15" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D15,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D15,'HEX GEN BACKEND'!G:G,0)),D15)</f>
-        <v>0000010</v>
+        <v>0000000</v>
       </c>
       <c r="O15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="P15" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F15,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F15,'HEX GEN BACKEND'!H:H,0)),F15)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="R15" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H15,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H15,'HEX GEN BACKEND'!I:I,0)),H15)</f>
-        <v>0000000</v>
+        <v>0000011</v>
       </c>
       <c r="S15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="U15" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001010000010100000001000000000</v>
+        <v>01000000000000010000010100000011</v>
       </c>
       <c r="W15" s="21" t="str">
         <f t="shared" si="2"/>
@@ -2865,7 +2861,7 @@
       </c>
       <c r="X15" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="Y15" s="21" t="str">
         <f t="shared" si="4"/>
@@ -2873,7 +2869,7 @@
       </c>
       <c r="Z15" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>1010</v>
+        <v>0001</v>
       </c>
       <c r="AA15" s="21" t="str">
         <f t="shared" si="6"/>
@@ -2881,7 +2877,7 @@
       </c>
       <c r="AB15" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0101</v>
       </c>
       <c r="AC15" s="21" t="str">
         <f t="shared" si="8"/>
@@ -2889,7 +2885,7 @@
       </c>
       <c r="AD15" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="AF15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W15,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2897,7 +2893,7 @@
       </c>
       <c r="AG15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y15,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2905,7 +2901,7 @@
       </c>
       <c r="AI15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA15,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2913,7 +2909,7 @@
       </c>
       <c r="AK15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AL15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC15,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2921,11 +2917,11 @@
       </c>
       <c r="AM15" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AO15" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>4A0A0200</v>
+        <v>40010503</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
@@ -2936,69 +2932,69 @@
         <v>16</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="E16" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="19" t="s">
         <v>68</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="J16" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>2A050301</v>
+        <v>48020483</v>
       </c>
       <c r="M16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C16,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0101</v>
+        <v>1001</v>
       </c>
       <c r="N16" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D16,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D16,'HEX GEN BACKEND'!G:G,0)),D16)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="O16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="P16" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F16,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F16,'HEX GEN BACKEND'!H:H,0)),F16)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="Q16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>10</v>
       </c>
       <c r="R16" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H16,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H16,'HEX GEN BACKEND'!I:I,0)),H16)</f>
-        <v>0000001</v>
+        <v>0000011</v>
       </c>
       <c r="S16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="U16" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00101010000001010000001100000001</v>
+        <v>01001000000000100000010010000011</v>
       </c>
       <c r="W16" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="X16" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="Y16" s="21" t="str">
         <f t="shared" si="4"/>
@@ -3006,7 +3002,7 @@
       </c>
       <c r="Z16" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0101</v>
+        <v>0010</v>
       </c>
       <c r="AA16" s="21" t="str">
         <f t="shared" si="6"/>
@@ -3014,23 +3010,23 @@
       </c>
       <c r="AB16" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0100</v>
       </c>
       <c r="AC16" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD16" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AF16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>8</v>
       </c>
       <c r="AH16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y16,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3038,7 +3034,7 @@
       </c>
       <c r="AI16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AJ16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA16,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3046,19 +3042,19 @@
       </c>
       <c r="AK16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AL16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM16" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AO16" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>2A050301</v>
+        <v>48020483</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
@@ -3069,77 +3065,77 @@
         <v>16</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>177</v>
+        <v>1</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>76</v>
+        <v>165</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J17" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>0A050302</v>
+        <v>56130180</v>
       </c>
       <c r="M17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C17,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0001</v>
+        <v>1010</v>
       </c>
       <c r="N17" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D17,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D17,'HEX GEN BACKEND'!G:G,0)),D17)</f>
-        <v>0000001</v>
+        <v>0000100</v>
       </c>
       <c r="O17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>11</v>
       </c>
       <c r="P17" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F17,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F17,'HEX GEN BACKEND'!H:H,0)),F17)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="Q17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>11</v>
       </c>
       <c r="R17" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H17,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H17,'HEX GEN BACKEND'!I:I,0)),H17)</f>
-        <v>0000010</v>
+        <v>0000000</v>
       </c>
       <c r="S17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="U17" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>00001010000001010000001100000010</v>
+        <v>01010110000100110000000110000000</v>
       </c>
       <c r="W17" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>0101</v>
       </c>
       <c r="X17" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1010</v>
+        <v>0110</v>
       </c>
       <c r="Y17" s="21" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="Z17" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0101</v>
+        <v>0011</v>
       </c>
       <c r="AA17" s="21" t="str">
         <f t="shared" si="6"/>
@@ -3147,31 +3143,31 @@
       </c>
       <c r="AB17" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="AC17" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD17" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AF17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>6</v>
       </c>
       <c r="AH17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA17,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3179,19 +3175,19 @@
       </c>
       <c r="AK17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM17" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO17" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>0A050302</v>
+        <v>56130180</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
@@ -3199,16 +3195,16 @@
         <v>53</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>98</v>
@@ -3217,26 +3213,26 @@
         <v>98</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="J18" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>4C040081</v>
+        <v>E2080000</v>
       </c>
       <c r="M18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C18,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>1100</v>
       </c>
       <c r="N18" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D18,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D18,'HEX GEN BACKEND'!G:G,0)),D18)</f>
-        <v>0000001</v>
+        <v>0000010</v>
       </c>
       <c r="O18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>01</v>
       </c>
       <c r="P18" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F18,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F18,'HEX GEN BACKEND'!H:H,0)),F18)</f>
@@ -3248,23 +3244,23 @@
       </c>
       <c r="R18" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H18,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H18,'HEX GEN BACKEND'!I:I,0)),H18)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="S18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="U18" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001100000001000000000010000001</v>
+        <v>11100010000010000000000000000000</v>
       </c>
       <c r="W18" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>1110</v>
       </c>
       <c r="X18" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1100</v>
+        <v>0010</v>
       </c>
       <c r="Y18" s="21" t="str">
         <f t="shared" si="4"/>
@@ -3272,7 +3268,7 @@
       </c>
       <c r="Z18" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AA18" s="21" t="str">
         <f t="shared" si="6"/>
@@ -3284,19 +3280,19 @@
       </c>
       <c r="AC18" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD18" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AF18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>E</v>
       </c>
       <c r="AG18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>2</v>
       </c>
       <c r="AH18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y18,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3304,7 +3300,7 @@
       </c>
       <c r="AI18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AJ18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA18,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3316,15 +3312,15 @@
       </c>
       <c r="AL18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM18" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO18" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>4C040081</v>
+        <v>E2080000</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
@@ -3332,72 +3328,72 @@
         <v>54</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="G19" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>67</v>
-      </c>
       <c r="H19" s="18" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="J19" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>48020282</v>
+        <v>E2040000</v>
       </c>
       <c r="M19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C19,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
+        <v>1100</v>
       </c>
       <c r="N19" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D19,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D19,'HEX GEN BACKEND'!G:G,0)),D19)</f>
-        <v>0000000</v>
+        <v>0000001</v>
       </c>
       <c r="O19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
+        <v>01</v>
       </c>
       <c r="P19" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(F19,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F19,'HEX GEN BACKEND'!H:H,0)),F19)</f>
-        <v>0000001</v>
+        <v>0000000</v>
       </c>
       <c r="Q19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
+        <v>00</v>
       </c>
       <c r="R19" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(H19,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H19,'HEX GEN BACKEND'!I:I,0)),H19)</f>
-        <v>0000010</v>
+        <v>0000000</v>
       </c>
       <c r="S19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
+        <v>00</v>
       </c>
       <c r="U19" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000100000001010000010</v>
+        <v>11100010000001000000000000000000</v>
       </c>
       <c r="W19" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>1110</v>
       </c>
       <c r="X19" s="21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="Y19" s="21" t="str">
         <f t="shared" si="4"/>
@@ -3405,7 +3401,7 @@
       </c>
       <c r="Z19" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="AA19" s="21" t="str">
         <f t="shared" si="6"/>
@@ -3413,23 +3409,23 @@
       </c>
       <c r="AB19" s="21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AC19" s="21" t="str">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD19" s="21" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AF19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>E</v>
       </c>
       <c r="AG19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y19,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3437,7 +3433,7 @@
       </c>
       <c r="AI19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AJ19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA19,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3445,19 +3441,19 @@
       </c>
       <c r="AK19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM19" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO19" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>48020282</v>
+        <v>E2040000</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
@@ -3467,130 +3463,116 @@
       <c r="B20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J20" s="13" t="str">
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>38010302</v>
-      </c>
-      <c r="M20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C20,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0111</v>
-      </c>
-      <c r="N20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N20" s="21">
         <f>IF(ISNUMBER(MATCH(D20,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D20,'HEX GEN BACKEND'!G:G,0)),D20)</f>
-        <v>0000000</v>
-      </c>
-      <c r="O20" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="O20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
-      </c>
-      <c r="P20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P20" s="21">
         <f>IF(ISNUMBER(MATCH(F20,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F20,'HEX GEN BACKEND'!H:H,0)),F20)</f>
-        <v>0000001</v>
-      </c>
-      <c r="Q20" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
-      </c>
-      <c r="R20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="21">
         <f>IF(ISNUMBER(MATCH(H20,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H20,'HEX GEN BACKEND'!I:I,0)),H20)</f>
-        <v>0000010</v>
-      </c>
-      <c r="S20" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="S20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
-      </c>
-      <c r="U20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U20" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>00111000000000010000001100000010</v>
-      </c>
-      <c r="W20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W20" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>0011</v>
-      </c>
-      <c r="X20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X20" s="21" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="Y20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y20" s="21" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Z20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z20" s="21" t="e">
         <f t="shared" si="5"/>
-        <v>0001</v>
-      </c>
-      <c r="AA20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA20" s="21" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AB20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB20" s="21" t="e">
         <f t="shared" si="7"/>
-        <v>0011</v>
-      </c>
-      <c r="AC20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC20" s="21" t="e">
         <f t="shared" si="8"/>
-        <v>0000</v>
-      </c>
-      <c r="AD20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AD20" s="21" t="e">
         <f t="shared" si="9"/>
-        <v>0010</v>
-      </c>
-      <c r="AF20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AG20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AH20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AJ20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AM20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AM20" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AO20" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO20" s="21" t="e">
         <f t="shared" si="10"/>
-        <v>38010302</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
@@ -3600,130 +3582,116 @@
       <c r="B21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="J21" s="13" t="str">
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>48020282</v>
-      </c>
-      <c r="M21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C21,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1001</v>
-      </c>
-      <c r="N21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N21" s="21">
         <f>IF(ISNUMBER(MATCH(D21,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D21,'HEX GEN BACKEND'!G:G,0)),D21)</f>
-        <v>0000000</v>
-      </c>
-      <c r="O21" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="O21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
-      </c>
-      <c r="P21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P21" s="21">
         <f>IF(ISNUMBER(MATCH(F21,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F21,'HEX GEN BACKEND'!H:H,0)),F21)</f>
-        <v>0000001</v>
-      </c>
-      <c r="Q21" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
-      </c>
-      <c r="R21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R21" s="21">
         <f>IF(ISNUMBER(MATCH(H21,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H21,'HEX GEN BACKEND'!I:I,0)),H21)</f>
-        <v>0000010</v>
-      </c>
-      <c r="S21" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="S21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
-      </c>
-      <c r="U21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U21" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000100000001010000010</v>
-      </c>
-      <c r="W21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W21" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="X21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X21" s="21" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="Y21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y21" s="21" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Z21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z21" s="21" t="e">
         <f t="shared" si="5"/>
-        <v>0010</v>
-      </c>
-      <c r="AA21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA21" s="21" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AB21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB21" s="21" t="e">
         <f t="shared" si="7"/>
-        <v>0010</v>
-      </c>
-      <c r="AC21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC21" s="21" t="e">
         <f t="shared" si="8"/>
-        <v>1000</v>
-      </c>
-      <c r="AD21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AD21" s="21" t="e">
         <f t="shared" si="9"/>
-        <v>0010</v>
-      </c>
-      <c r="AF21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AG21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AH21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AJ21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AM21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AM21" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AO21" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO21" s="21" t="e">
         <f t="shared" si="10"/>
-        <v>48020282</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
@@ -3733,130 +3701,116 @@
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="13" t="str">
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>36010301</v>
-      </c>
-      <c r="M22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C22,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>0110</v>
-      </c>
-      <c r="N22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N22" s="21">
         <f>IF(ISNUMBER(MATCH(D22,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D22,'HEX GEN BACKEND'!G:G,0)),D22)</f>
-        <v>0000000</v>
-      </c>
-      <c r="O22" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="O22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>11</v>
-      </c>
-      <c r="P22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P22" s="21">
         <f>IF(ISNUMBER(MATCH(F22,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F22,'HEX GEN BACKEND'!H:H,0)),F22)</f>
-        <v>0000001</v>
-      </c>
-      <c r="Q22" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
-      </c>
-      <c r="R22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R22" s="21">
         <f>IF(ISNUMBER(MATCH(H22,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H22,'HEX GEN BACKEND'!I:I,0)),H22)</f>
-        <v>0000001</v>
-      </c>
-      <c r="S22" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="S22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>10</v>
-      </c>
-      <c r="U22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U22" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>00110110000000010000001100000001</v>
-      </c>
-      <c r="W22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W22" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>0011</v>
-      </c>
-      <c r="X22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X22" s="21" t="e">
         <f t="shared" si="3"/>
-        <v>0110</v>
-      </c>
-      <c r="Y22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y22" s="21" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Z22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z22" s="21" t="e">
         <f t="shared" si="5"/>
-        <v>0001</v>
-      </c>
-      <c r="AA22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA22" s="21" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AB22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB22" s="21" t="e">
         <f t="shared" si="7"/>
-        <v>0011</v>
-      </c>
-      <c r="AC22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC22" s="21" t="e">
         <f t="shared" si="8"/>
-        <v>0000</v>
-      </c>
-      <c r="AD22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AD22" s="21" t="e">
         <f t="shared" si="9"/>
-        <v>0001</v>
-      </c>
-      <c r="AF22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AG22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AH22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AJ22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AM22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AM22" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AO22" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO22" s="21" t="e">
         <f t="shared" si="10"/>
-        <v>36010301</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -3866,130 +3820,116 @@
       <c r="B23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="13" t="str">
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>563B2C81</v>
-      </c>
-      <c r="M23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C23,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1010</v>
-      </c>
-      <c r="N23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N23" s="21">
         <f>IF(ISNUMBER(MATCH(D23,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D23,'HEX GEN BACKEND'!G:G,0)),D23)</f>
-        <v>0001110</v>
-      </c>
-      <c r="O23" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="O23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>11</v>
-      </c>
-      <c r="P23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P23" s="21">
         <f>IF(ISNUMBER(MATCH(F23,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F23,'HEX GEN BACKEND'!H:H,0)),F23)</f>
-        <v>0010110</v>
-      </c>
-      <c r="Q23" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>11</v>
-      </c>
-      <c r="R23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R23" s="21">
         <f>IF(ISNUMBER(MATCH(H23,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H23,'HEX GEN BACKEND'!I:I,0)),H23)</f>
-        <v>0000001</v>
-      </c>
-      <c r="S23" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="S23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
-      </c>
-      <c r="U23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U23" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>01010110001110110010110010000001</v>
-      </c>
-      <c r="W23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W23" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>0101</v>
-      </c>
-      <c r="X23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X23" s="21" t="e">
         <f t="shared" si="3"/>
-        <v>0110</v>
-      </c>
-      <c r="Y23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y23" s="21" t="e">
         <f t="shared" si="4"/>
-        <v>0011</v>
-      </c>
-      <c r="Z23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z23" s="21" t="e">
         <f t="shared" si="5"/>
-        <v>1011</v>
-      </c>
-      <c r="AA23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA23" s="21" t="e">
         <f t="shared" si="6"/>
-        <v>0010</v>
-      </c>
-      <c r="AB23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB23" s="21" t="e">
         <f t="shared" si="7"/>
-        <v>1100</v>
-      </c>
-      <c r="AC23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC23" s="21" t="e">
         <f t="shared" si="8"/>
-        <v>1000</v>
-      </c>
-      <c r="AD23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AD23" s="21" t="e">
         <f t="shared" si="9"/>
-        <v>0001</v>
-      </c>
-      <c r="AF23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AG23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AH23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AI23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>B</v>
-      </c>
-      <c r="AJ23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AK23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AL23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AM23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AM23" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AO23" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO23" s="21" t="e">
         <f t="shared" si="10"/>
-        <v>563B2C81</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -3997,132 +3937,118 @@
         <v>59</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="J24" s="13" t="str">
+        <v>16</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="13" t="e">
         <f t="shared" si="0"/>
-        <v>E2040000</v>
-      </c>
-      <c r="M24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C24,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1100</v>
-      </c>
-      <c r="N24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N24" s="21">
         <f>IF(ISNUMBER(MATCH(D24,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D24,'HEX GEN BACKEND'!G:G,0)),D24)</f>
-        <v>0000001</v>
-      </c>
-      <c r="O24" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="O24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(E24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>01</v>
-      </c>
-      <c r="P24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P24" s="21">
         <f>IF(ISNUMBER(MATCH(F24,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(F24,'HEX GEN BACKEND'!H:H,0)),F24)</f>
-        <v>0000000</v>
-      </c>
-      <c r="Q24" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(G24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
-      </c>
-      <c r="R24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="R24" s="21">
         <f>IF(ISNUMBER(MATCH(H24,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(H24,'HEX GEN BACKEND'!I:I,0)),H24)</f>
-        <v>0000000</v>
-      </c>
-      <c r="S24" s="21" t="str">
+        <v>0</v>
+      </c>
+      <c r="S24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(I24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>00</v>
-      </c>
-      <c r="U24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="U24" s="21" t="e">
         <f t="shared" si="1"/>
-        <v>11100010000001000000000000000000</v>
-      </c>
-      <c r="W24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W24" s="21" t="e">
         <f t="shared" si="2"/>
-        <v>1110</v>
-      </c>
-      <c r="X24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X24" s="21" t="e">
         <f t="shared" si="3"/>
-        <v>0010</v>
-      </c>
-      <c r="Y24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y24" s="21" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Z24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z24" s="21" t="e">
         <f t="shared" si="5"/>
-        <v>0100</v>
-      </c>
-      <c r="AA24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA24" s="21" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AB24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB24" s="21" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AC24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC24" s="21" t="e">
         <f t="shared" si="8"/>
-        <v>0000</v>
-      </c>
-      <c r="AD24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AD24" s="21" t="e">
         <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
-      <c r="AF24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>E</v>
-      </c>
-      <c r="AG24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AH24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AJ24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AL24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AM24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AM24" s="21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AD24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AO24" s="21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AO24" s="21" t="e">
         <f t="shared" si="10"/>
-        <v>E2040000</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
@@ -13146,7 +13072,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13159,7 +13085,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$A:$A</xm:f>
@@ -13170,7 +13096,7 @@
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$D:$D</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E101 G2:G101 I2:I101</xm:sqref>
+          <xm:sqref>I2:I101 G2:G101 E2:E101</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
DIVISION done but minor bugs
</commit_message>
<xml_diff>
--- a/INSTRUCTIONS/Binary Instructions.xlsx
+++ b/INSTRUCTIONS/Binary Instructions.xlsx
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +2496,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>78</v>
@@ -2518,11 +2518,11 @@
       </c>
       <c r="J11" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>620C0000</v>
+        <v>020C0000</v>
       </c>
       <c r="M11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C11,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1100</v>
+        <v>0000</v>
       </c>
       <c r="N11" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D11,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D11,'HEX GEN BACKEND'!G:G,0)),D11)</f>
@@ -2550,11 +2550,11 @@
       </c>
       <c r="U11" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01100010000011000000000000000000</v>
+        <v>00000010000011000000000000000000</v>
       </c>
       <c r="W11" s="21" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="X11" s="21" t="str">
         <f t="shared" si="3"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="AF11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG11" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2618,7 +2618,7 @@
       </c>
       <c r="AO11" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>620C0000</v>
+        <v>020C0000</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
@@ -9013,7 +9013,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="49" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D60" s="50" t="s">
         <v>137</v>
@@ -9035,11 +9035,11 @@
       </c>
       <c r="J60" s="22" t="str">
         <f t="shared" si="19"/>
-        <v>62200000</v>
+        <v>02200000</v>
       </c>
       <c r="M60" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C60,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1100</v>
+        <v>0000</v>
       </c>
       <c r="N60" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D60,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D60,'HEX GEN BACKEND'!G:G,0)),D60)</f>
@@ -9067,11 +9067,11 @@
       </c>
       <c r="U60" s="21" t="str">
         <f t="shared" si="1"/>
-        <v>01100010001000000000000000000000</v>
+        <v>00000010001000000000000000000000</v>
       </c>
       <c r="W60" s="21" t="str">
         <f t="shared" si="11"/>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="X60" s="21" t="str">
         <f t="shared" si="12"/>
@@ -9103,7 +9103,7 @@
       </c>
       <c r="AF60" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W60,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG60" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X60,'HEX GEN BACKEND'!L:L,0))</f>
@@ -9135,7 +9135,7 @@
       </c>
       <c r="AO60" s="21" t="str">
         <f t="shared" si="10"/>
-        <v>62200000</v>
+        <v>02200000</v>
       </c>
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.25">
@@ -10077,7 +10077,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>139</v>
@@ -10099,11 +10099,11 @@
       </c>
       <c r="J68" s="22" t="str">
         <f t="shared" si="19"/>
-        <v>62280000</v>
+        <v>02280000</v>
       </c>
       <c r="M68" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(C68,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>1100</v>
+        <v>0000</v>
       </c>
       <c r="N68" s="21" t="str">
         <f>IF(ISNUMBER(MATCH(D68,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(D68,'HEX GEN BACKEND'!G:G,0)),D68)</f>
@@ -10131,11 +10131,11 @@
       </c>
       <c r="U68" s="21" t="str">
         <f t="shared" si="20"/>
-        <v>01100010001010000000000000000000</v>
+        <v>00000010001010000000000000000000</v>
       </c>
       <c r="W68" s="21" t="str">
         <f t="shared" si="11"/>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="X68" s="21" t="str">
         <f t="shared" si="12"/>
@@ -10167,7 +10167,7 @@
       </c>
       <c r="AF68" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W68,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG68" s="21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X68,'HEX GEN BACKEND'!L:L,0))</f>
@@ -10199,7 +10199,7 @@
       </c>
       <c r="AO68" s="21" t="str">
         <f t="shared" si="21"/>
-        <v>62280000</v>
+        <v>02280000</v>
       </c>
     </row>
     <row r="69" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>